<commit_message>
Updated the guide to datasets.xlsx
</commit_message>
<xml_diff>
--- a/06_guide_to_datasets.xlsx
+++ b/06_guide_to_datasets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d8c41f4a4675e5d/Documents/PhD/Thesis/Quantitative strand/social_rent_rdd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\IJHP_replication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="11_F25DC773A252ABDACC10480141D944465ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FF400C6-4C81-4864-830B-908B523D3826}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963D180C-EF54-4E2A-B8AA-3691F34D679F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
   <si>
     <t>File name</t>
   </si>
@@ -132,24 +132,6 @@
     <t>ONS: House price statistics for small areas (HPSSAs): Dataset 6 Number of residential property sales for administrative geographies</t>
   </si>
   <si>
-    <t>regionalgrossdomesticproductgdplocalauthorities.xlsx</t>
-  </si>
-  <si>
-    <t>GDP per capita</t>
-  </si>
-  <si>
-    <t>ONS: Regional gross domestic product: local authorities</t>
-  </si>
-  <si>
-    <t>MYEB1_detailed_population_estimates_series_UK_(2020_geog21).csv</t>
-  </si>
-  <si>
-    <t>Population growth</t>
-  </si>
-  <si>
-    <t>ONS: Population estimates and components of population change. detailed time series 2001 to 2020</t>
-  </si>
-  <si>
     <t>https://opendatacommunities.org/resource?uri=http%3A%2F%2Fopendatacommunities.org%2Fdata%2Fhouse-building%2Fstarts%2Ftenure</t>
   </si>
   <si>
@@ -159,12 +141,6 @@
     <t>https://www.ons.gov.uk/peoplepopulationandcommunity/housing/datasets/numberofresidentialpropertysalesfornationalandsubnationalgeographiesquarterlyrollingyearhpssadataset06</t>
   </si>
   <si>
-    <t>https://www.ons.gov.uk/economy/grossdomesticproductgdp/datasets/regionalgrossdomesticproductlocalauthorities</t>
-  </si>
-  <si>
-    <t>https://www.ons.gov.uk/peoplepopulationandcommunity/populationandmigration/populationestimates/datasets/populationestimatesforukenglandandwalesscotlandandnorthernireland</t>
-  </si>
-  <si>
     <t>https://www.gov.uk/government/statistical-data-sets/live-tables-on-affordable-housing-supply</t>
   </si>
   <si>
@@ -181,6 +157,87 @@
   </si>
   <si>
     <t>https://www.gov.uk/government/collections/private-registered-provider-social-housing-stock-in-england</t>
+  </si>
+  <si>
+    <t>Median earnings</t>
+  </si>
+  <si>
+    <t>ONS Median earnings</t>
+  </si>
+  <si>
+    <t>median_earnings.csv</t>
+  </si>
+  <si>
+    <t>https://www.ons.gov.uk/peoplepopulationandcommunity/housing/datasets/ratioofhousepricetoresidencebasedearningslowerquartileandmedian/current</t>
+  </si>
+  <si>
+    <t>ONS Household projections for England: 2018-based principal projection edition</t>
+  </si>
+  <si>
+    <t>Households total / Households change</t>
+  </si>
+  <si>
+    <t>2018basedhhpsprincipalprojection.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.ons.gov.uk/peoplepopulationandcommunity/populationandmigration/populationprojections/datasets/householdprojectionsforengland</t>
+  </si>
+  <si>
+    <t>Subnational estimates of dwellings by tenure, England, 2012 to 2021</t>
+  </si>
+  <si>
+    <t>Existing social housing supply</t>
+  </si>
+  <si>
+    <t>subnationaldwellingsbytenure2021.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.ons.gov.uk/peoplepopulationandcommunity/housing/datasets/subnationaldwellingstockbytenureestimates</t>
+  </si>
+  <si>
+    <t>2016_industry_employment.csv</t>
+  </si>
+  <si>
+    <t>2017_industry_employment.csv</t>
+  </si>
+  <si>
+    <t>2018_industry_employment.csv</t>
+  </si>
+  <si>
+    <t>2019_industry_employment.csv</t>
+  </si>
+  <si>
+    <t>2020_industry_employment.csv</t>
+  </si>
+  <si>
+    <t>Professional and financial employment</t>
+  </si>
+  <si>
+    <t>2016 Business Register and Employment Survey: Broad industrial group</t>
+  </si>
+  <si>
+    <t>2017 Business Register and Employment Survey: Broad industrial group</t>
+  </si>
+  <si>
+    <t>2018 Business Register and Employment Survey: Broad industrial group</t>
+  </si>
+  <si>
+    <t>2019 Business Register and Employment Survey: Broad industrial group</t>
+  </si>
+  <si>
+    <t>2020 Business Register and Employment Survey: Broad industrial group</t>
+  </si>
+  <si>
+    <t>Nomis data query</t>
+  </si>
+  <si>
+    <t>ONS: Population estimates - local authority based by single year of age</t>
+  </si>
+  <si>
+    <t>Over 65s percentage</t>
+  </si>
+  <si>
+    <t>la_all_ages.csv</t>
   </si>
 </sst>
 </file>
@@ -508,25 +565,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="107.5546875" customWidth="1"/>
+    <col min="1" max="1" width="107.54296875" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.36328125" customWidth="1"/>
     <col min="4" max="4" width="69" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -534,7 +591,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -543,7 +600,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -557,10 +614,10 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -574,10 +631,10 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -591,10 +648,10 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -608,10 +665,10 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -625,10 +682,10 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -642,10 +699,10 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -659,10 +716,10 @@
         <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -676,10 +733,10 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -693,10 +750,10 @@
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -710,12 +767,12 @@
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -727,10 +784,10 @@
         <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -744,10 +801,10 @@
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -761,10 +818,10 @@
         <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -778,41 +835,160 @@
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C16" s="2">
-        <v>44887</v>
+        <v>45455</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C17" s="2">
-        <v>44967</v>
+        <v>45455</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="2">
+        <v>45455</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="2">
+        <v>45455</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="2">
+        <v>45455</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="2">
+        <v>45455</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="2">
+        <v>45455</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="2">
+        <v>45455</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="2">
+        <v>45455</v>
+      </c>
+      <c r="D24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>